<commit_message>
Partially fixed component evaluation pipeline, minor issues remain
</commit_message>
<xml_diff>
--- a/3_Component_Results/CONSTR/Data/naive_err/AR2_50_9_qoq_errors_first_eval.xlsx
+++ b/3_Component_Results/CONSTR/Data/naive_err/AR2_50_9_qoq_errors_first_eval.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Q0</t>
   </si>
@@ -26,6 +26,120 @@
   </si>
   <si>
     <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>Q7</t>
+  </si>
+  <si>
+    <t>Q8</t>
+  </si>
+  <si>
+    <t>Q9</t>
+  </si>
+  <si>
+    <t>2010-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2010-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2011-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2011-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2012-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2012-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2013-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2013-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2014-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2014-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2015-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2015-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2016-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2016-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2017-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2017-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2018-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2018-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2018-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2018-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2019-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2019-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2019-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2019-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2020-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2020-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2020-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2020-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2021-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2021-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2021-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2021-10-01 00:00:00_diff</t>
   </si>
   <si>
     <t>2022-01-01 00:00:00_diff</t>
@@ -428,13 +542,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:11">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,176 +561,1503 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2">
+        <v>1.602065061688767</v>
+      </c>
+      <c r="C2">
+        <v>3.04003431312337</v>
+      </c>
+      <c r="D2">
+        <v>-5.938674847989947</v>
+      </c>
+      <c r="E2">
+        <v>0.711740365345836</v>
+      </c>
+      <c r="F2">
+        <v>1.004187453457734</v>
+      </c>
+      <c r="G2">
+        <v>-1.571576459402547</v>
+      </c>
+      <c r="H2">
+        <v>1.677040253876188</v>
+      </c>
+      <c r="I2">
+        <v>1.413579134973207</v>
+      </c>
+      <c r="J2">
+        <v>-1.1970418117026</v>
+      </c>
+      <c r="K2">
+        <v>1.063997643474595</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>-5.964533143146513</v>
+      </c>
+      <c r="C3">
+        <v>1.176669382365755</v>
+      </c>
+      <c r="D3">
+        <v>1.257909854851463</v>
+      </c>
+      <c r="E3">
+        <v>-1.316511037723468</v>
+      </c>
+      <c r="F3">
+        <v>1.953767573022166</v>
+      </c>
+      <c r="G3">
+        <v>1.68470952429612</v>
+      </c>
+      <c r="H3">
+        <v>-0.9267333470265362</v>
+      </c>
+      <c r="I3">
+        <v>1.335090377852552</v>
+      </c>
+      <c r="J3">
+        <v>2.689117542185831</v>
+      </c>
+      <c r="K3">
+        <v>-1.30947372129706</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>-0.1912892836565094</v>
+      </c>
+      <c r="C4">
+        <v>-1.883142166085352</v>
+      </c>
+      <c r="D4">
+        <v>2.40342068983337</v>
+      </c>
+      <c r="E4">
+        <v>1.59145081812635</v>
+      </c>
+      <c r="F4">
+        <v>-1.01940872675969</v>
+      </c>
+      <c r="G4">
+        <v>1.347470452837819</v>
+      </c>
+      <c r="H4">
+        <v>2.663069105302687</v>
+      </c>
+      <c r="I4">
+        <v>-1.341821941620366</v>
+      </c>
+      <c r="J4">
+        <v>-1.778606615788304</v>
+      </c>
+      <c r="K4">
+        <v>0.3811183547683571</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>2.451560068375472</v>
+      </c>
+      <c r="C5">
+        <v>1.631250807461972</v>
+      </c>
+      <c r="D5">
+        <v>-1.136384491199137</v>
+      </c>
+      <c r="E5">
+        <v>1.288882177974849</v>
+      </c>
+      <c r="F5">
+        <v>2.617100029502487</v>
+      </c>
+      <c r="G5">
+        <v>-1.404849577761434</v>
+      </c>
+      <c r="H5">
+        <v>-1.838157574296937</v>
+      </c>
+      <c r="I5">
+        <v>0.3239328258660771</v>
+      </c>
+      <c r="J5">
+        <v>-3.12412545836584</v>
+      </c>
+      <c r="K5">
+        <v>4.41214789954688</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>-0.6713463558411743</v>
+      </c>
+      <c r="C6">
+        <v>1.456403131754811</v>
+      </c>
+      <c r="D6">
+        <v>2.410179470697346</v>
+      </c>
+      <c r="E6">
+        <v>-1.416845180694781</v>
+      </c>
+      <c r="F6">
+        <v>-1.843726900463117</v>
+      </c>
+      <c r="G6">
+        <v>0.2763261090784467</v>
+      </c>
+      <c r="H6">
+        <v>-3.157964936554458</v>
+      </c>
+      <c r="I6">
+        <v>4.381938073622721</v>
+      </c>
+      <c r="J6">
+        <v>0.8314869420358898</v>
+      </c>
+      <c r="K6">
+        <v>-0.8417899989297971</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>2.558311128377992</v>
+      </c>
+      <c r="C7">
+        <v>-1.61703114258315</v>
+      </c>
+      <c r="D7">
+        <v>-1.787905310785899</v>
+      </c>
+      <c r="E7">
+        <v>0.3172458133749849</v>
+      </c>
+      <c r="F7">
+        <v>-3.165321551741034</v>
+      </c>
+      <c r="G7">
+        <v>4.394211510218005</v>
+      </c>
+      <c r="H7">
+        <v>0.8470970267896389</v>
+      </c>
+      <c r="I7">
+        <v>-0.8314115959935573</v>
+      </c>
+      <c r="J7">
+        <v>-1.203936152349081</v>
+      </c>
+      <c r="K7">
+        <v>1.797584205437971</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>-1.000583923879169</v>
+      </c>
+      <c r="C8">
+        <v>0.3330464057515683</v>
+      </c>
+      <c r="D8">
+        <v>-3.501808595795778</v>
+      </c>
+      <c r="E8">
+        <v>4.312478024421555</v>
+      </c>
+      <c r="F8">
+        <v>0.7516536693615905</v>
+      </c>
+      <c r="G8">
+        <v>-0.9702593289485597</v>
+      </c>
+      <c r="H8">
+        <v>-1.326653518038879</v>
+      </c>
+      <c r="I8">
+        <v>1.677947847921885</v>
+      </c>
+      <c r="J8">
+        <v>0.6973247173158894</v>
+      </c>
+      <c r="K8">
+        <v>-1.59689593491947</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>-4.035980535359728</v>
+      </c>
+      <c r="C9">
+        <v>4.281733970436962</v>
+      </c>
+      <c r="D9">
+        <v>1.060050001689662</v>
+      </c>
+      <c r="E9">
+        <v>-0.8800767286206297</v>
+      </c>
+      <c r="F9">
+        <v>-1.237312706125463</v>
+      </c>
+      <c r="G9">
+        <v>1.813922149940158</v>
+      </c>
+      <c r="H9">
+        <v>0.8182811675798158</v>
+      </c>
+      <c r="I9">
+        <v>-1.480935762477904</v>
+      </c>
+      <c r="J9">
+        <v>-1.83101885996277</v>
+      </c>
+      <c r="K9">
+        <v>2.400816341023468</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>0.0297336039017963</v>
+      </c>
+      <c r="C10">
+        <v>-1.023359033907779</v>
+      </c>
+      <c r="D10">
+        <v>-0.869267155944665</v>
+      </c>
+      <c r="E10">
+        <v>1.851321450814572</v>
+      </c>
+      <c r="F10">
+        <v>0.8671359181158229</v>
+      </c>
+      <c r="G10">
+        <v>-1.373961301725209</v>
+      </c>
+      <c r="H10">
+        <v>-1.745011347826217</v>
+      </c>
+      <c r="I10">
+        <v>2.48271734209359</v>
+      </c>
+      <c r="J10">
+        <v>0.3007856631840057</v>
+      </c>
+      <c r="K10">
+        <v>-0.2444340177882403</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>0.131091278350679</v>
+      </c>
+      <c r="C11">
+        <v>1.642837495150672</v>
+      </c>
+      <c r="D11">
+        <v>0.7042417988596263</v>
+      </c>
+      <c r="E11">
+        <v>-1.286160639479628</v>
+      </c>
+      <c r="F11">
+        <v>-1.752246416917782</v>
+      </c>
+      <c r="G11">
+        <v>2.452807261485723</v>
+      </c>
+      <c r="H11">
+        <v>0.2993245036869432</v>
+      </c>
+      <c r="I11">
+        <v>-0.2505920205412158</v>
+      </c>
+      <c r="J11">
+        <v>-1.732235314432763</v>
+      </c>
+      <c r="K11">
+        <v>0.07591040760561318</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>0.3636878794241752</v>
+      </c>
+      <c r="C12">
+        <v>-1.480850976740869</v>
+      </c>
+      <c r="D12">
+        <v>-1.623235328945376</v>
+      </c>
+      <c r="E12">
+        <v>2.44452898475904</v>
+      </c>
+      <c r="F12">
+        <v>0.2650830578612836</v>
+      </c>
+      <c r="G12">
+        <v>-0.2464089501930713</v>
+      </c>
+      <c r="H12">
+        <v>-1.734903978400189</v>
+      </c>
+      <c r="I12">
+        <v>0.06709218995131727</v>
+      </c>
+      <c r="J12">
+        <v>0.997638680340651</v>
+      </c>
+      <c r="K12">
+        <v>0.9225122398852474</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>-1.133793310742067</v>
+      </c>
+      <c r="C13">
+        <v>2.396506616762759</v>
+      </c>
+      <c r="D13">
+        <v>0.1334929590812335</v>
+      </c>
+      <c r="E13">
+        <v>-0.2424074626040421</v>
+      </c>
+      <c r="F13">
+        <v>-1.759145924760854</v>
+      </c>
+      <c r="G13">
+        <v>0.02504033491206281</v>
+      </c>
+      <c r="H13">
+        <v>0.9671701603683858</v>
+      </c>
+      <c r="I13">
+        <v>0.8917581291730856</v>
+      </c>
+      <c r="J13">
+        <v>-1.540527083993024</v>
+      </c>
+      <c r="K13">
+        <v>-0.07648217258257672</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>-0.5855037078925832</v>
+      </c>
+      <c r="C14">
+        <v>-0.3500558685895692</v>
+      </c>
+      <c r="D14">
+        <v>-1.531013389883137</v>
+      </c>
+      <c r="E14">
+        <v>0.01571105264383821</v>
+      </c>
+      <c r="F14">
+        <v>0.9649422761041804</v>
+      </c>
+      <c r="G14">
+        <v>0.9369298121875916</v>
+      </c>
+      <c r="H14">
+        <v>-1.512292777968344</v>
+      </c>
+      <c r="I14">
+        <v>-0.05264886514247225</v>
+      </c>
+      <c r="J14">
+        <v>-0.3382994898529339</v>
+      </c>
+      <c r="K14">
+        <v>-0.7236222237478239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>-1.175388651429754</v>
+      </c>
+      <c r="C15">
+        <v>-0.1162368441329322</v>
+      </c>
+      <c r="D15">
+        <v>0.8744227152943851</v>
+      </c>
+      <c r="E15">
+        <v>0.9386878373742611</v>
+      </c>
+      <c r="F15">
+        <v>-1.550010950011433</v>
+      </c>
+      <c r="G15">
+        <v>-0.09737356966267874</v>
+      </c>
+      <c r="H15">
+        <v>-0.3721388207766118</v>
+      </c>
+      <c r="I15">
+        <v>-0.759534533284935</v>
+      </c>
+      <c r="J15">
+        <v>-1.377648804732524</v>
+      </c>
+      <c r="K15">
+        <v>1.550224523917756</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>0.3552134418812914</v>
+      </c>
+      <c r="C16">
+        <v>0.7362320718836142</v>
+      </c>
+      <c r="D16">
+        <v>-1.343310833598577</v>
+      </c>
+      <c r="E16">
+        <v>-0.08797516315622933</v>
+      </c>
+      <c r="F16">
+        <v>-0.3851574201046055</v>
+      </c>
+      <c r="G16">
+        <v>-0.7240937595609835</v>
+      </c>
+      <c r="H16">
+        <v>-1.353035944078457</v>
+      </c>
+      <c r="I16">
+        <v>1.568165001629739</v>
+      </c>
+      <c r="J16">
+        <v>-0.6267843906273527</v>
+      </c>
+      <c r="K16">
+        <v>-0.05459425183377231</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>-1.183907986438387</v>
+      </c>
+      <c r="C17">
+        <v>0.05700775802553448</v>
+      </c>
+      <c r="D17">
+        <v>-0.4358955283822323</v>
+      </c>
+      <c r="E17">
+        <v>-0.71141671765916</v>
+      </c>
+      <c r="F17">
+        <v>-1.319553654061151</v>
+      </c>
+      <c r="G17">
+        <v>1.582133422844289</v>
+      </c>
+      <c r="H17">
+        <v>-0.6110836150814311</v>
+      </c>
+      <c r="I17">
+        <v>-0.03539985811346014</v>
+      </c>
+      <c r="J17">
+        <v>-3.537205679518259</v>
+      </c>
+      <c r="K17">
+        <v>4.784984400263594</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>0.3341125450935086</v>
+      </c>
+      <c r="C18">
+        <v>-0.3508114577303035</v>
+      </c>
+      <c r="D18">
+        <v>-0.8760990133289467</v>
+      </c>
+      <c r="E18">
+        <v>-1.365850698791239</v>
+      </c>
+      <c r="F18">
+        <v>1.549247401710418</v>
+      </c>
+      <c r="G18">
+        <v>-0.6723735983230095</v>
+      </c>
+      <c r="H18">
+        <v>-0.09041745470805995</v>
+      </c>
+      <c r="I18">
+        <v>-3.588418648010414</v>
+      </c>
+      <c r="J18">
+        <v>4.731285395698713</v>
+      </c>
+      <c r="K18">
+        <v>0.9037942130729857</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>-0.683652730876144</v>
+      </c>
+      <c r="C19">
+        <v>-0.8805789581820997</v>
+      </c>
+      <c r="D19">
+        <v>-1.196102773105657</v>
+      </c>
+      <c r="E19">
+        <v>1.602640335434466</v>
+      </c>
+      <c r="F19">
+        <v>-0.6155938371719847</v>
+      </c>
+      <c r="G19">
+        <v>-0.01273115972318184</v>
+      </c>
+      <c r="H19">
+        <v>-3.517909015219086</v>
+      </c>
+      <c r="I19">
+        <v>4.800101007260582</v>
+      </c>
+      <c r="J19">
+        <v>0.9744931146455251</v>
+      </c>
+      <c r="K19">
+        <v>-0.2997701464397722</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>-1.058735208844254</v>
+      </c>
+      <c r="C20">
+        <v>-1.386999006280221</v>
+      </c>
+      <c r="D20">
+        <v>1.549332777060623</v>
+      </c>
+      <c r="E20">
+        <v>-0.7099199683210056</v>
+      </c>
+      <c r="F20">
+        <v>-0.1254456407988778</v>
+      </c>
+      <c r="G20">
+        <v>-3.615789618673908</v>
+      </c>
+      <c r="H20">
+        <v>4.701809843085441</v>
+      </c>
+      <c r="I20">
+        <v>0.8730718431514469</v>
+      </c>
+      <c r="J20">
+        <v>-0.4001795282862969</v>
+      </c>
+      <c r="K20">
+        <v>4.109053225130578</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>-1.648727594640484</v>
+      </c>
+      <c r="C21">
+        <v>1.462507427632228</v>
+      </c>
+      <c r="D21">
+        <v>-0.6721476239130408</v>
+      </c>
+      <c r="E21">
+        <v>-0.1515068856602781</v>
+      </c>
+      <c r="F21">
+        <v>-3.647989130500227</v>
+      </c>
+      <c r="G21">
+        <v>4.682660325192878</v>
+      </c>
+      <c r="H21">
+        <v>0.8517292273033832</v>
+      </c>
+      <c r="I21">
+        <v>-0.4233051323841132</v>
+      </c>
+      <c r="J21">
+        <v>4.086760318251222</v>
+      </c>
+      <c r="K21">
+        <v>-0.2304354376121681</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>1.06218499483979</v>
+      </c>
+      <c r="C22">
+        <v>-0.8852389630105697</v>
+      </c>
+      <c r="D22">
+        <v>-0.0558786353357319</v>
+      </c>
+      <c r="E22">
+        <v>-3.70716334433386</v>
+      </c>
+      <c r="F22">
+        <v>4.594578303184172</v>
+      </c>
+      <c r="G22">
+        <v>0.8144047504659724</v>
+      </c>
+      <c r="H22">
+        <v>-0.4699199680661165</v>
+      </c>
+      <c r="I22">
+        <v>4.029691742782072</v>
+      </c>
+      <c r="J22">
+        <v>-0.2815567415983687</v>
+      </c>
+      <c r="K22">
+        <v>-0.6884749412588014</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23">
+        <v>-1.340115292431498</v>
+      </c>
+      <c r="C23">
+        <v>-0.353195832274076</v>
+      </c>
+      <c r="D23">
+        <v>-3.440436284661193</v>
+      </c>
+      <c r="E23">
+        <v>4.643106980273811</v>
+      </c>
+      <c r="F23">
+        <v>0.7820040214703584</v>
+      </c>
+      <c r="G23">
+        <v>-0.4192578927116719</v>
+      </c>
+      <c r="H23">
+        <v>4.075771321973281</v>
+      </c>
+      <c r="I23">
+        <v>-0.2560267305039844</v>
+      </c>
+      <c r="J23">
+        <v>-0.6552992021731622</v>
+      </c>
+      <c r="K23">
+        <v>0.1039294925726918</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>-0.05068199948299379</v>
+      </c>
+      <c r="C24">
+        <v>-3.231842090227025</v>
+      </c>
+      <c r="D24">
+        <v>4.599304726625893</v>
+      </c>
+      <c r="E24">
+        <v>0.8602096247968869</v>
+      </c>
+      <c r="F24">
+        <v>-0.3248604380118332</v>
+      </c>
+      <c r="G24">
+        <v>4.132638447728763</v>
+      </c>
+      <c r="H24">
+        <v>-0.1886245657752045</v>
+      </c>
+      <c r="I24">
+        <v>-0.5822688371598701</v>
+      </c>
+      <c r="J24">
+        <v>0.1720074739919267</v>
+      </c>
+      <c r="K24">
+        <v>-1.600325323120769</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25">
+        <v>-3.377437691350778</v>
+      </c>
+      <c r="C25">
+        <v>4.529096781379431</v>
+      </c>
+      <c r="D25">
+        <v>0.9789225614280446</v>
+      </c>
+      <c r="E25">
+        <v>-0.2924999983369396</v>
+      </c>
+      <c r="F25">
+        <v>4.142616210569781</v>
+      </c>
+      <c r="G25">
+        <v>-0.1468258169145158</v>
+      </c>
+      <c r="H25">
+        <v>-0.5455501989603571</v>
+      </c>
+      <c r="I25">
+        <v>0.2017583108656847</v>
+      </c>
+      <c r="J25">
+        <v>-1.566681958130874</v>
+      </c>
+      <c r="K25">
+        <v>2.139513935359049</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>4.801485318762561</v>
+      </c>
+      <c r="C26">
+        <v>0.913267839525427</v>
+      </c>
+      <c r="D26">
+        <v>-0.3319556201640653</v>
+      </c>
+      <c r="E26">
+        <v>4.183318683871708</v>
+      </c>
+      <c r="F26">
+        <v>-0.1443451787808422</v>
+      </c>
+      <c r="G26">
+        <v>-0.5496348297789975</v>
+      </c>
+      <c r="H26">
+        <v>0.2104665134444246</v>
+      </c>
+      <c r="I26">
+        <v>-1.561198728680113</v>
+      </c>
+      <c r="J26">
+        <v>2.142823683514327</v>
+      </c>
+      <c r="K26">
+        <v>0.7899716644520379</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>-0.3717561422703723</v>
+      </c>
+      <c r="C27">
+        <v>-0.8791019322052089</v>
+      </c>
+      <c r="D27">
+        <v>4.723422806035984</v>
+      </c>
+      <c r="E27">
+        <v>-0.2434644514457658</v>
+      </c>
+      <c r="F27">
+        <v>-0.7089467587897555</v>
+      </c>
+      <c r="G27">
+        <v>0.2580654574225746</v>
+      </c>
+      <c r="H27">
+        <v>-1.577742318730656</v>
+      </c>
+      <c r="I27">
+        <v>2.092202407356854</v>
+      </c>
+      <c r="J27">
+        <v>0.7711425963514449</v>
+      </c>
+      <c r="K27">
+        <v>1.026220945753324</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>1.317909765080107</v>
+      </c>
+      <c r="C28">
+        <v>3.797168329633632</v>
+      </c>
+      <c r="D28">
+        <v>-0.4269883030396099</v>
+      </c>
+      <c r="E28">
+        <v>-0.3270824085490708</v>
+      </c>
+      <c r="F28">
+        <v>0.2092499475065616</v>
+      </c>
+      <c r="G28">
+        <v>-1.610904003810268</v>
+      </c>
+      <c r="H28">
+        <v>2.171877149624135</v>
+      </c>
+      <c r="I28">
+        <v>0.8014493027578454</v>
+      </c>
+      <c r="J28">
+        <v>1.044988844403852</v>
+      </c>
+      <c r="K28">
+        <v>-0.08570940516299164</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <v>4.868353134686993</v>
+      </c>
+      <c r="C29">
+        <v>-0.5057144731676827</v>
+      </c>
+      <c r="D29">
+        <v>-0.6382104669498487</v>
+      </c>
+      <c r="E29">
+        <v>0.3608051673070891</v>
+      </c>
+      <c r="F29">
+        <v>-1.587973328183784</v>
+      </c>
+      <c r="G29">
+        <v>2.104050342715349</v>
+      </c>
+      <c r="H29">
+        <v>0.8131736491205633</v>
+      </c>
+      <c r="I29">
+        <v>1.051925846892968</v>
+      </c>
+      <c r="J29">
+        <v>-0.1020868192923516</v>
+      </c>
+      <c r="K29">
+        <v>1.631323344741358</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30">
+        <v>1.161480604400402</v>
+      </c>
+      <c r="C30">
+        <v>0.2507779444996481</v>
+      </c>
+      <c r="D30">
+        <v>-0.5697470420513719</v>
+      </c>
+      <c r="E30">
+        <v>-1.516687622035615</v>
+      </c>
+      <c r="F30">
+        <v>2.3589959397342</v>
+      </c>
+      <c r="G30">
+        <v>0.6652987897018862</v>
+      </c>
+      <c r="H30">
+        <v>1.009361028138957</v>
+      </c>
+      <c r="I30">
+        <v>-0.05633312782496203</v>
+      </c>
+      <c r="J30">
+        <v>1.60647940076914</v>
+      </c>
+      <c r="K30">
+        <v>1.777570978320599</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31">
+        <v>-0.6228858727657893</v>
+      </c>
+      <c r="C31">
+        <v>0.4094712395283026</v>
+      </c>
+      <c r="D31">
+        <v>-1.394739097106807</v>
+      </c>
+      <c r="E31">
+        <v>2.215146711838581</v>
+      </c>
+      <c r="F31">
+        <v>0.91640298512986</v>
+      </c>
+      <c r="G31">
+        <v>1.188024152733261</v>
+      </c>
+      <c r="H31">
+        <v>0.01952723792658473</v>
+      </c>
+      <c r="I31">
+        <v>1.748443717015282</v>
+      </c>
+      <c r="J31">
+        <v>1.92733335770093</v>
+      </c>
+      <c r="K31">
+        <v>1.893240954502724</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32">
+        <v>0.2696417855765004</v>
+      </c>
+      <c r="C32">
+        <v>-1.614289770673047</v>
+      </c>
+      <c r="D32">
+        <v>2.347735810496459</v>
+      </c>
+      <c r="E32">
+        <v>0.921189511792661</v>
+      </c>
+      <c r="F32">
+        <v>1.105398905390152</v>
+      </c>
+      <c r="G32">
+        <v>0.02979362249283102</v>
+      </c>
+      <c r="H32">
+        <v>1.752413480389771</v>
+      </c>
+      <c r="I32">
+        <v>1.895710647137968</v>
+      </c>
+      <c r="J32">
+        <v>1.880529444923089</v>
+      </c>
+      <c r="K32">
+        <v>0.8280725750199738</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>-0.13114668368188</v>
+      </c>
+      <c r="C33">
+        <v>1.742666631567946</v>
+      </c>
+      <c r="D33">
+        <v>0.5711375823114974</v>
+      </c>
+      <c r="E33">
+        <v>1.482408709799302</v>
+      </c>
+      <c r="F33">
+        <v>-0.03207898350142768</v>
+      </c>
+      <c r="G33">
+        <v>1.599008421811034</v>
+      </c>
+      <c r="H33">
+        <v>1.962174432224697</v>
+      </c>
+      <c r="I33">
+        <v>1.882496678171399</v>
+      </c>
+      <c r="J33">
+        <v>0.7708382429261704</v>
+      </c>
+      <c r="K33">
+        <v>1.964522524714165</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34">
         <v>1.827023400069947</v>
       </c>
-      <c r="C2">
+      <c r="C34">
         <v>0.4888028508193502</v>
       </c>
-      <c r="D2">
+      <c r="D34">
         <v>1.471596344594558</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
+      <c r="E34">
+        <v>0.007347806326601258</v>
+      </c>
+      <c r="F34">
+        <v>1.588860911059396</v>
+      </c>
+      <c r="G34">
+        <v>1.947337590876925</v>
+      </c>
+      <c r="H34">
+        <v>1.89204969391759</v>
+      </c>
+      <c r="I34">
+        <v>0.7728960159151987</v>
+      </c>
+      <c r="J34">
+        <v>1.958518439087574</v>
+      </c>
+      <c r="K34">
+        <v>1.295963201187878</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35">
         <v>0.06190938385428302</v>
       </c>
-      <c r="C3">
+      <c r="C35">
         <v>2.26017545783639</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
+      <c r="D35">
+        <v>-0.2558836427411291</v>
+      </c>
+      <c r="E35">
+        <v>1.246425756096891</v>
+      </c>
+      <c r="F35">
+        <v>2.066184569109413</v>
+      </c>
+      <c r="G35">
+        <v>1.859708481389941</v>
+      </c>
+      <c r="H35">
+        <v>0.6119859734886953</v>
+      </c>
+      <c r="I35">
+        <v>1.910929136767185</v>
+      </c>
+      <c r="J35">
+        <v>1.255730557254227</v>
+      </c>
+      <c r="K35">
+        <v>0.9072349556365198</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36">
         <v>2.750952690361402</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
+      <c r="C36">
+        <v>-0.5685323890927088</v>
+      </c>
+      <c r="D36">
+        <v>1.099336473843246</v>
+      </c>
+      <c r="E36">
+        <v>2.109713815817977</v>
+      </c>
+      <c r="F36">
+        <v>1.76264761573322</v>
+      </c>
+      <c r="G36">
+        <v>0.5186442976695476</v>
+      </c>
+      <c r="H36">
+        <v>1.861806893584042</v>
+      </c>
+      <c r="I36">
+        <v>1.182766877946806</v>
+      </c>
+      <c r="J36">
+        <v>0.8320577075686965</v>
+      </c>
+      <c r="K36">
+        <v>0.7243956030543357</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37">
         <v>0.7320287013142677</v>
       </c>
-      <c r="C5">
+      <c r="C37">
         <v>1.522302341005567</v>
       </c>
-      <c r="D5">
+      <c r="D37">
         <v>1.467338125109618</v>
       </c>
-      <c r="E5">
+      <c r="E37">
         <v>1.793638825175652</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
+      <c r="F37">
+        <v>0.677999698236624</v>
+      </c>
+      <c r="G37">
+        <v>1.741859006123216</v>
+      </c>
+      <c r="H37">
+        <v>1.118463222389436</v>
+      </c>
+      <c r="I37">
+        <v>0.8458034752539987</v>
+      </c>
+      <c r="J37">
+        <v>0.6898869152123258</v>
+      </c>
+      <c r="K37">
+        <v>0.473162559883601</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38">
         <v>1.9795770604465</v>
       </c>
-      <c r="C6">
+      <c r="C38">
         <v>1.392536339603099</v>
       </c>
-      <c r="D6">
+      <c r="D38">
         <v>1.481510914913067</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
+      <c r="E38">
+        <v>0.5495882858316863</v>
+      </c>
+      <c r="F38">
+        <v>1.646265717678995</v>
+      </c>
+      <c r="G38">
+        <v>0.9624354823172134</v>
+      </c>
+      <c r="H38">
+        <v>0.6946493953545967</v>
+      </c>
+      <c r="I38">
+        <v>0.5552724956881216</v>
+      </c>
+      <c r="J38">
+        <v>0.3325484856772042</v>
+      </c>
+      <c r="K38">
+        <v>0.4721920549197476</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39">
         <v>1.30090756340108</v>
       </c>
-      <c r="C7">
+      <c r="C39">
         <v>1.963500078556037</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
+      <c r="D39">
+        <v>0.4445961937514334</v>
+      </c>
+      <c r="E39">
+        <v>1.596344060894952</v>
+      </c>
+      <c r="F39">
+        <v>1.02220498890233</v>
+      </c>
+      <c r="G39">
+        <v>0.7092913393505274</v>
+      </c>
+      <c r="H39">
+        <v>0.5601932978503645</v>
+      </c>
+      <c r="I39">
+        <v>0.3499962282384746</v>
+      </c>
+      <c r="J39">
+        <v>0.4879072232831797</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40">
         <v>2.012737994557474</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
+      <c r="C40">
+        <v>0.7403123565715917</v>
+      </c>
+      <c r="D40">
+        <v>1.433818452601332</v>
+      </c>
+      <c r="E40">
+        <v>0.9497534119557898</v>
+      </c>
+      <c r="F40">
+        <v>0.7298655388265476</v>
+      </c>
+      <c r="G40">
+        <v>0.5258654170934298</v>
+      </c>
+      <c r="H40">
+        <v>0.3090287986856384</v>
+      </c>
+      <c r="I40">
+        <v>0.4635204163707518</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41">
         <v>0.8535918672211444</v>
       </c>
-      <c r="C9">
+      <c r="C41">
         <v>1.782613822028589</v>
       </c>
-      <c r="D9">
+      <c r="D41">
         <v>0.7889205787030562</v>
       </c>
-      <c r="E9">
+      <c r="E41">
         <v>0.6461210271256811</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
+      <c r="F41">
+        <v>0.5323553410679266</v>
+      </c>
+      <c r="G41">
+        <v>0.2768565178553412</v>
+      </c>
+      <c r="H41">
+        <v>0.4210073694104794</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42">
         <v>1.972402569862437</v>
       </c>
-      <c r="C10">
+      <c r="C42">
         <v>0.8237969262448452</v>
       </c>
-      <c r="D10">
+      <c r="D42">
         <v>0.4993394432980468</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
+      <c r="E42">
+        <v>0.4591344678357677</v>
+      </c>
+      <c r="F42">
+        <v>0.2243478747645702</v>
+      </c>
+      <c r="G42">
+        <v>0.3483362424206175</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43">
         <v>0.796001625707733</v>
       </c>
-      <c r="C11">
+      <c r="C43">
         <v>0.9151352642427935</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
+      <c r="D43">
+        <v>0.3687495555490187</v>
+      </c>
+      <c r="E43">
+        <v>0.1821182294781293</v>
+      </c>
+      <c r="F43">
+        <v>0.3937388773370095</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44">
         <v>1.082826669985442</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13">
+      <c r="C44">
+        <v>0.3935261511656301</v>
+      </c>
+      <c r="D44">
+        <v>0.06540634303695037</v>
+      </c>
+      <c r="E44">
+        <v>0.3242309254185909</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45">
         <v>0.573129683809814</v>
       </c>
-      <c r="C13">
+      <c r="C45">
         <v>0.1945252858301101</v>
       </c>
-      <c r="D13">
+      <c r="D45">
         <v>0.2603721808367071</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14">
+    <row r="46" spans="1:11">
+      <c r="A46" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46">
         <v>0.1824667929082922</v>
       </c>
-      <c r="C14">
+      <c r="C46">
         <v>0.4481552108942597</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15">
+    <row r="47" spans="1:11">
+      <c r="A47" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47">
         <v>0.3345343741504182</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1" t="s">
-        <v>18</v>
+    <row r="48" spans="1:11">
+      <c r="A48" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>